<commit_message>
Deploying to gh-pages from  @ ebe4073d9ea32d40643f7692ca212675714cb022 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/16.1.1.1.xlsx
+++ b/en/downloads/data-excel/16.1.1.1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t>Кыргызская Республика</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>16.1.1.1 Mortality from attacks per 100,000 population</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -793,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -807,7 +810,7 @@
     <col min="4" max="4" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="38.25">
+    <row r="1" spans="1:21" ht="38.25">
       <c r="A1" s="12" t="s">
         <v>14</v>
       </c>
@@ -821,7 +824,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:21">
       <c r="A2" s="13" t="s">
         <v>15</v>
       </c>
@@ -835,11 +838,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="15.75" thickBot="1">
+    <row r="3" spans="1:21" ht="15.75" thickBot="1">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:20" ht="15.75" thickBot="1">
+    <row r="4" spans="1:21" ht="15.75" thickBot="1">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -900,8 +903,11 @@
       <c r="T4" s="38">
         <v>2022</v>
       </c>
+      <c r="U4" s="38">
+        <v>2023</v>
+      </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:21">
       <c r="A5" s="15" t="s">
         <v>17</v>
       </c>
@@ -962,8 +968,11 @@
       <c r="T5" s="40">
         <v>2.6</v>
       </c>
+      <c r="U5" s="40">
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:21">
       <c r="A6" s="16" t="s">
         <v>18</v>
       </c>
@@ -1024,8 +1033,11 @@
       <c r="T6" s="39">
         <v>1.8</v>
       </c>
+      <c r="U6" s="39">
+        <v>0.3</v>
+      </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:21">
       <c r="A7" s="16" t="s">
         <v>19</v>
       </c>
@@ -1086,8 +1098,11 @@
       <c r="T7" s="39">
         <v>2.6</v>
       </c>
+      <c r="U7" s="39">
+        <v>0.4</v>
+      </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:21">
       <c r="A8" s="16" t="s">
         <v>20</v>
       </c>
@@ -1148,8 +1163,11 @@
       <c r="T8" s="39">
         <v>1.9</v>
       </c>
+      <c r="U8" s="39">
+        <v>0.4</v>
+      </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:21">
       <c r="A9" s="16" t="s">
         <v>21</v>
       </c>
@@ -1210,8 +1228,11 @@
       <c r="T9" s="39">
         <v>3.9</v>
       </c>
+      <c r="U9" s="39">
+        <v>3.2</v>
+      </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:21">
       <c r="A10" s="16" t="s">
         <v>22</v>
       </c>
@@ -1272,8 +1293,11 @@
       <c r="T10" s="39">
         <v>3.2</v>
       </c>
+      <c r="U10" s="39">
+        <v>0.6</v>
+      </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:21">
       <c r="A11" s="16" t="s">
         <v>23</v>
       </c>
@@ -1334,8 +1358,11 @@
       <c r="T11" s="39">
         <v>3.3</v>
       </c>
+      <c r="U11" s="39" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:21">
       <c r="A12" s="16" t="s">
         <v>24</v>
       </c>
@@ -1396,8 +1423,11 @@
       <c r="T12" s="39">
         <v>2.5</v>
       </c>
+      <c r="U12" s="39">
+        <v>0.6</v>
+      </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:21">
       <c r="A13" s="17" t="s">
         <v>25</v>
       </c>
@@ -1458,8 +1488,11 @@
       <c r="T13" s="39">
         <v>1.9</v>
       </c>
+      <c r="U13" s="39">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="14" spans="1:20" ht="15.75" thickBot="1">
+    <row r="14" spans="1:21" ht="15.75" thickBot="1">
       <c r="A14" s="20" t="s">
         <v>26</v>
       </c>
@@ -1520,8 +1553,11 @@
       <c r="T14" s="41">
         <v>2.5</v>
       </c>
+      <c r="U14" s="41">
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:21">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="10"/>

</xml_diff>